<commit_message>
Se agrega actualizacion automatica de productos al insertar uno
</commit_message>
<xml_diff>
--- a/reporte_inventario.xlsx
+++ b/reporte_inventario.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,96 +467,96 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Sofá modular</t>
+          <t>Mesa comedor 6p</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D2" t="n">
-        <v>799.99</v>
+        <v>549.5</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>unidad</t>
+          <t>juego</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Sala</t>
+          <t>Comedor</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Mesa comedor 6p</t>
+          <t>Silla giratoria</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D3" t="n">
-        <v>549.5</v>
+        <v>129.99</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>juego</t>
+          <t>unidad</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Comedor</t>
+          <t>Oficina</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
+        <v>5</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Juego de terraza</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
         <v>3</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Silla giratoria</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>20</v>
-      </c>
       <c r="D4" t="n">
-        <v>129.99</v>
+        <v>899.9</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>unidad</t>
+          <t>juego</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Oficina</t>
+          <t>Exteriores</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Cama Queen</t>
+          <t>Lámpara de pie</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D5" t="n">
-        <v>699</v>
+        <v>85.75</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -565,76 +565,76 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Dormitorio</t>
+          <t>Sala</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Juego de terraza</t>
+          <t>Escritorio ejecutivo</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D6" t="n">
-        <v>899.9</v>
+        <v>399</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>juego</t>
+          <t>unidad</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Exteriores</t>
+          <t>Oficina</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Lámpara de pie</t>
+          <t>Velador doble</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D7" t="n">
-        <v>85.75</v>
+        <v>120</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>unidad</t>
+          <t>par</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Sala</t>
+          <t>Dormitorio</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Escritorio ejecutivo</t>
+          <t>Zapatero zeta</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D8" t="n">
-        <v>399</v>
+        <v>120</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -643,28 +643,28 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Oficina</t>
+          <t>Dormitorio</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Velador doble</t>
+          <t>Cama Queen</t>
         </is>
       </c>
       <c r="C9" t="n">
         <v>10</v>
       </c>
       <c r="D9" t="n">
-        <v>120</v>
+        <v>699</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>par</t>
+          <t>unidad</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -675,53 +675,339 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Silla plegable</t>
+          <t>Zapatera</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="D10" t="n">
-        <v>45.99</v>
+        <v>250</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>unidad</t>
+          <t>juego</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Exteriores</t>
+          <t>Sala</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
+        <v>1</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Sofá modular</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
         <v>10</v>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="D11" t="n">
+        <v>799.99</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>unidad</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Sala</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>9</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Silla plegable</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>21</v>
+      </c>
+      <c r="D12" t="n">
+        <v>45.99</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>unidad</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Exteriores</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>10</v>
+      </c>
+      <c r="B13" t="inlineStr">
         <is>
           <t>Repisa flotante</t>
         </is>
       </c>
-      <c r="C11" t="n">
+      <c r="C13" t="n">
         <v>30</v>
       </c>
-      <c r="D11" t="n">
+      <c r="D13" t="n">
         <v>29.95</v>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="E13" t="inlineStr">
         <is>
           <t>pieza</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Oficina</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>$%&amp;</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>2</v>
+      </c>
+      <c r="D14" t="n">
+        <v>2</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>par</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Comedor</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Ropero Estela</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D15" t="n">
+        <v>300</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>unidad</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Dormitorio</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Ropero choco</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>23</v>
+      </c>
+      <c r="D16" t="n">
+        <v>235</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>unidad</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Dormitorio</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Comoda Lunaria</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>23</v>
+      </c>
+      <c r="D17" t="n">
+        <v>230</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>unidad</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Dormitorio</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>PRUEBA123</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>212</v>
+      </c>
+      <c r="D18" t="n">
+        <v>23</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>par</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Comedor</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>prueba4</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>23</v>
+      </c>
+      <c r="D19" t="n">
+        <v>23</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>unidad</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
         <is>
           <t>Sala</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Prueba5</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>1232</v>
+      </c>
+      <c r="D20" t="n">
+        <v>231</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>juego</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Oficina</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>21</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>hola</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>23</v>
+      </c>
+      <c r="D21" t="n">
+        <v>234</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>par</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Oficina</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>hola123</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>123</v>
+      </c>
+      <c r="D22" t="n">
+        <v>123</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>juego</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Oficina</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Se ordenan ascendemente los productos de los reportes en pdf y excel
</commit_message>
<xml_diff>
--- a/reporte_inventario.xlsx
+++ b/reporte_inventario.xlsx
@@ -467,96 +467,96 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Mesa comedor 6p</t>
+          <t>Sofá modular</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D2" t="n">
-        <v>549.5</v>
+        <v>799.99</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>juego</t>
+          <t>unidad</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Comedor</t>
+          <t>Sala</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Silla giratoria</t>
+          <t>Mesa comedor 6p</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D3" t="n">
-        <v>129.99</v>
+        <v>549.5</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>unidad</t>
+          <t>juego</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Oficina</t>
+          <t>Comedor</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Juego de terraza</t>
+          <t>Silla giratoria</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="D4" t="n">
-        <v>899.9</v>
+        <v>129.99</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>juego</t>
+          <t>unidad</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Exteriores</t>
+          <t>Oficina</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Lámpara de pie</t>
+          <t>Cama Queen</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D5" t="n">
-        <v>85.75</v>
+        <v>699</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -565,76 +565,76 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Sala</t>
+          <t>Dormitorio</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Escritorio ejecutivo</t>
+          <t>Juego de terraza</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D6" t="n">
-        <v>399</v>
+        <v>899.9</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>unidad</t>
+          <t>juego</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Oficina</t>
+          <t>Exteriores</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Velador doble</t>
+          <t>Lámpara de pie</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D7" t="n">
-        <v>120</v>
+        <v>85.75</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>par</t>
+          <t>unidad</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Dormitorio</t>
+          <t>Sala</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Zapatero zeta</t>
+          <t>Escritorio ejecutivo</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D8" t="n">
-        <v>120</v>
+        <v>399</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -643,28 +643,28 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Dormitorio</t>
+          <t>Oficina</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Cama Queen</t>
+          <t>Velador doble</t>
         </is>
       </c>
       <c r="C9" t="n">
         <v>10</v>
       </c>
       <c r="D9" t="n">
-        <v>699</v>
+        <v>120</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>unidad</t>
+          <t>par</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -675,105 +675,105 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Zapatera</t>
+          <t>Silla plegable</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="D10" t="n">
-        <v>250</v>
+        <v>45.99</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>juego</t>
+          <t>unidad</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Sala</t>
+          <t>Exteriores</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Sofá modular</t>
+          <t>Repisa flotante</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="D11" t="n">
-        <v>799.99</v>
+        <v>29.95</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>unidad</t>
+          <t>pieza</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Sala</t>
+          <t>Oficina</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Silla plegable</t>
+          <t>Zapatera</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="D12" t="n">
-        <v>45.99</v>
+        <v>250</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>unidad</t>
+          <t>juego</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Exteriores</t>
+          <t>Sala</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Repisa flotante</t>
+          <t>Zapatero zeta</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="D13" t="n">
-        <v>29.95</v>
+        <v>120</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>pieza</t>
+          <t>unidad</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Oficina</t>
+          <t>Dormitorio</t>
         </is>
       </c>
     </row>
@@ -961,22 +961,22 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>hola</t>
+          <t>hola123</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>23</v>
+        <v>123</v>
       </c>
       <c r="D21" t="n">
-        <v>234</v>
+        <v>123</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>par</t>
+          <t>juego</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -987,22 +987,22 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>hola123</t>
+          <t>hola</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>123</v>
+        <v>23</v>
       </c>
       <c r="D22" t="n">
-        <v>123</v>
+        <v>234</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>juego</t>
+          <t>par</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">

</xml_diff>

<commit_message>
Se refactoriza la logica de eliminar producto con mostrar el producto
</commit_message>
<xml_diff>
--- a/reporte_inventario.xlsx
+++ b/reporte_inventario.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -727,287 +727,27 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Zapatera</t>
+          <t>Velador mediano de roble</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D12" t="n">
-        <v>250</v>
+        <v>140</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>juego</t>
+          <t>unidad</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Sala</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Zapatero zeta</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>2</v>
-      </c>
-      <c r="D13" t="n">
-        <v>120</v>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>unidad</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
           <t>Dormitorio</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>13</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>$%&amp;</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>2</v>
-      </c>
-      <c r="D14" t="n">
-        <v>2</v>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>par</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>Comedor</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>14</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Ropero Estela</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>2</v>
-      </c>
-      <c r="D15" t="n">
-        <v>300</v>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>unidad</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>Dormitorio</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>15</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Ropero choco</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
-        <v>23</v>
-      </c>
-      <c r="D16" t="n">
-        <v>235</v>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>unidad</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>Dormitorio</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>16</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Comoda Lunaria</t>
-        </is>
-      </c>
-      <c r="C17" t="n">
-        <v>23</v>
-      </c>
-      <c r="D17" t="n">
-        <v>230</v>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>unidad</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>Dormitorio</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>17</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>PRUEBA123</t>
-        </is>
-      </c>
-      <c r="C18" t="n">
-        <v>212</v>
-      </c>
-      <c r="D18" t="n">
-        <v>23</v>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>par</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>Comedor</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>18</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>prueba4</t>
-        </is>
-      </c>
-      <c r="C19" t="n">
-        <v>23</v>
-      </c>
-      <c r="D19" t="n">
-        <v>23</v>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>unidad</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>Sala</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>19</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Prueba5</t>
-        </is>
-      </c>
-      <c r="C20" t="n">
-        <v>1232</v>
-      </c>
-      <c r="D20" t="n">
-        <v>231</v>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>juego</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>Oficina</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>20</v>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>hola123</t>
-        </is>
-      </c>
-      <c r="C21" t="n">
-        <v>123</v>
-      </c>
-      <c r="D21" t="n">
-        <v>123</v>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>juego</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>Oficina</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>21</v>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>hola</t>
-        </is>
-      </c>
-      <c r="C22" t="n">
-        <v>23</v>
-      </c>
-      <c r="D22" t="n">
-        <v>234</v>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>par</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>Oficina</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Documentacion en mostrar inventario
</commit_message>
<xml_diff>
--- a/reporte_inventario.xlsx
+++ b/reporte_inventario.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -727,287 +727,27 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Zapatera</t>
+          <t>Velador mediano de roble</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D12" t="n">
-        <v>250</v>
+        <v>140</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>juego</t>
+          <t>unidad</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Sala</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Zapatero zeta</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>2</v>
-      </c>
-      <c r="D13" t="n">
-        <v>120</v>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>unidad</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
           <t>Dormitorio</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>13</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>$%&amp;</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>2</v>
-      </c>
-      <c r="D14" t="n">
-        <v>2</v>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>par</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>Comedor</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>14</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Ropero Estela</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>2</v>
-      </c>
-      <c r="D15" t="n">
-        <v>300</v>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>unidad</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>Dormitorio</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>15</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Ropero choco</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
-        <v>23</v>
-      </c>
-      <c r="D16" t="n">
-        <v>235</v>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>unidad</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>Dormitorio</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>16</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Comoda Lunaria</t>
-        </is>
-      </c>
-      <c r="C17" t="n">
-        <v>23</v>
-      </c>
-      <c r="D17" t="n">
-        <v>230</v>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>unidad</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>Dormitorio</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>17</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>PRUEBA123</t>
-        </is>
-      </c>
-      <c r="C18" t="n">
-        <v>212</v>
-      </c>
-      <c r="D18" t="n">
-        <v>23</v>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>par</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>Comedor</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>18</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>prueba4</t>
-        </is>
-      </c>
-      <c r="C19" t="n">
-        <v>23</v>
-      </c>
-      <c r="D19" t="n">
-        <v>23</v>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>unidad</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>Sala</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>19</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Prueba5</t>
-        </is>
-      </c>
-      <c r="C20" t="n">
-        <v>1232</v>
-      </c>
-      <c r="D20" t="n">
-        <v>231</v>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>juego</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>Oficina</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>20</v>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>hola123</t>
-        </is>
-      </c>
-      <c r="C21" t="n">
-        <v>123</v>
-      </c>
-      <c r="D21" t="n">
-        <v>123</v>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>juego</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>Oficina</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>21</v>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>hola</t>
-        </is>
-      </c>
-      <c r="C22" t="n">
-        <v>23</v>
-      </c>
-      <c r="D22" t="n">
-        <v>234</v>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>par</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>Oficina</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Bug 11 corregido - formato UX legible para excel
</commit_message>
<xml_diff>
--- a/reporte_inventario.xlsx
+++ b/reporte_inventario.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -28,13 +28,22 @@
     <font>
       <b val="1"/>
     </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="004CAF50"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -55,10 +64,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -425,281 +440,478 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="35" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="18" customWidth="1" min="6" max="6"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Reporte generado el 18/05/2025 a las 20:33</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B2" s="2" t="inlineStr">
         <is>
           <t>Nombre</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C2" s="2" t="inlineStr">
         <is>
           <t>Cantidad</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D2" s="2" t="inlineStr">
         <is>
           <t>Precio</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E2" s="2" t="inlineStr">
         <is>
           <t>Unidad</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F2" s="2" t="inlineStr">
         <is>
           <t>Categoría</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
+    <row r="3">
+      <c r="A3" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Sofá modular</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>HPe</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>50</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>50</v>
+      </c>
+      <c r="E3" s="3" t="inlineStr">
+        <is>
+          <t>pieza</t>
+        </is>
+      </c>
+      <c r="F3" s="3" t="inlineStr">
+        <is>
+          <t>Sala</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>Cama Queen</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="D2" t="n">
-        <v>799.99</v>
-      </c>
-      <c r="E2" t="inlineStr">
+      <c r="D4" s="3" t="n">
+        <v>699</v>
+      </c>
+      <c r="E4" s="3" t="inlineStr">
         <is>
           <t>unidad</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F4" s="3" t="inlineStr">
+        <is>
+          <t>Dormitorio</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>Juego de terraza</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>899.9</v>
+      </c>
+      <c r="E5" s="3" t="inlineStr">
+        <is>
+          <t>juego</t>
+        </is>
+      </c>
+      <c r="F5" s="3" t="inlineStr">
+        <is>
+          <t>Exteriores</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>Lámpara de pie</t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>85.75</v>
+      </c>
+      <c r="E6" s="3" t="inlineStr">
+        <is>
+          <t>unidad</t>
+        </is>
+      </c>
+      <c r="F6" s="3" t="inlineStr">
         <is>
           <t>Sala</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Mesa comedor 6p</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
+    <row r="7">
+      <c r="A7" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="D3" t="n">
-        <v>549.5</v>
-      </c>
-      <c r="E3" t="inlineStr">
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>Escritorio ejecutivo</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>10000000000</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>399</v>
+      </c>
+      <c r="E7" s="3" t="inlineStr">
+        <is>
+          <t>unidad</t>
+        </is>
+      </c>
+      <c r="F7" s="3" t="inlineStr">
+        <is>
+          <t>Oficina</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="inlineStr">
+        <is>
+          <t>Velador doble</t>
+        </is>
+      </c>
+      <c r="C8" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="D8" s="3" t="n">
+        <v>120</v>
+      </c>
+      <c r="E8" s="3" t="inlineStr">
+        <is>
+          <t>par</t>
+        </is>
+      </c>
+      <c r="F8" s="3" t="inlineStr">
+        <is>
+          <t>Dormitorio</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>Silla comedor</t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="n">
+        <v>32000</v>
+      </c>
+      <c r="D9" s="3" t="n">
+        <v>45.999</v>
+      </c>
+      <c r="E9" s="3" t="inlineStr">
+        <is>
+          <t>unidad</t>
+        </is>
+      </c>
+      <c r="F9" s="3" t="inlineStr">
+        <is>
+          <t>Exteriores</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>Sall</t>
+        </is>
+      </c>
+      <c r="C10" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="D10" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3" t="inlineStr">
+        <is>
+          <t>unidad</t>
+        </is>
+      </c>
+      <c r="F10" s="3" t="inlineStr">
+        <is>
+          <t>Comedor</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>asda</t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="D11" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="E11" s="3" t="inlineStr">
+        <is>
+          <t>unidad</t>
+        </is>
+      </c>
+      <c r="F11" s="3" t="inlineStr">
+        <is>
+          <t>Comedor</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t>bf12</t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="D12" s="3" t="n">
+        <v>25.55</v>
+      </c>
+      <c r="E12" s="3" t="inlineStr">
         <is>
           <t>juego</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F12" s="3" t="inlineStr">
+        <is>
+          <t>Sala</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3" t="inlineStr">
+        <is>
+          <t>...Afsbhehuhfhfdjkdsfjksjksdfjkfdjsfdhjsfd</t>
+        </is>
+      </c>
+      <c r="C13" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="D13" s="3" t="n">
+        <v>111</v>
+      </c>
+      <c r="E13" s="3" t="inlineStr">
+        <is>
+          <t>kit</t>
+        </is>
+      </c>
+      <c r="F13" s="3" t="inlineStr">
         <is>
           <t>Comedor</t>
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Silla giratoria</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>20</v>
-      </c>
-      <c r="D4" t="n">
-        <v>129.99</v>
-      </c>
-      <c r="E4" t="inlineStr">
+    <row r="14">
+      <c r="A14" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" s="3" t="inlineStr">
+        <is>
+          <t>pan</t>
+        </is>
+      </c>
+      <c r="C14" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="D14" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="E14" s="3" t="inlineStr">
         <is>
           <t>unidad</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F14" s="3" t="inlineStr">
+        <is>
+          <t>Comedor</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" s="3" t="inlineStr">
+        <is>
+          <t>Hola</t>
+        </is>
+      </c>
+      <c r="C15" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="D15" s="3" t="n">
+        <v>123</v>
+      </c>
+      <c r="E15" s="3" t="inlineStr">
+        <is>
+          <t>unidad</t>
+        </is>
+      </c>
+      <c r="F15" s="3" t="inlineStr">
+        <is>
+          <t>Comedor</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" s="3" t="inlineStr">
+        <is>
+          <t>Hola 123</t>
+        </is>
+      </c>
+      <c r="C16" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="D16" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="E16" s="3" t="inlineStr">
+        <is>
+          <t>unidad</t>
+        </is>
+      </c>
+      <c r="F16" s="3" t="inlineStr">
+        <is>
+          <t>Sala</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" s="3" t="inlineStr">
+        <is>
+          <t>La Potona</t>
+        </is>
+      </c>
+      <c r="C17" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="D17" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="E17" s="3" t="inlineStr">
+        <is>
+          <t>juego</t>
+        </is>
+      </c>
+      <c r="F17" s="3" t="inlineStr">
         <is>
           <t>Oficina</t>
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Cama Queen</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>10</v>
-      </c>
-      <c r="D5" t="n">
-        <v>699</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>unidad</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Dormitorio</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Juego de terraza</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>3</v>
-      </c>
-      <c r="D6" t="n">
-        <v>899.9</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>juego</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Exteriores</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Lámpara de pie</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>15</v>
-      </c>
-      <c r="D7" t="n">
-        <v>85.75</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>unidad</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
+    <row r="18">
+      <c r="A18" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" s="3" t="inlineStr">
+        <is>
+          <t>Vas A Cáer Chuponsito</t>
+        </is>
+      </c>
+      <c r="C18" s="3" t="n">
+        <v>1212</v>
+      </c>
+      <c r="D18" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="E18" s="3" t="inlineStr">
+        <is>
+          <t>par</t>
+        </is>
+      </c>
+      <c r="F18" s="3" t="inlineStr">
         <is>
           <t>Sala</t>
         </is>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Escritorio ejecutivo</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>8</v>
-      </c>
-      <c r="D8" t="n">
-        <v>399</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>unidad</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Oficina</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Velador doble</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>10</v>
-      </c>
-      <c r="D9" t="n">
-        <v>120</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>par</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Dormitorio</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Silla plegable</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>21</v>
-      </c>
-      <c r="D10" t="n">
-        <v>45.99</v>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>unidad</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Exteriores</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Bug 12 corregido - Caracteres especiales luego de digitar caracteres alfabeticos
</commit_message>
<xml_diff>
--- a/reporte_inventario.xlsx
+++ b/reporte_inventario.xlsx
@@ -440,7 +440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,7 +456,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Reporte generado el 18/05/2025 a las 20:33</t>
+          <t>Reporte generado el 18/05/2025 a las 20:52</t>
         </is>
       </c>
     </row>
@@ -680,7 +680,7 @@
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
-          <t>Sall</t>
+          <t>Juego Sala - 123</t>
         </is>
       </c>
       <c r="C10" s="3" t="n">
@@ -706,23 +706,23 @@
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>asda</t>
+          <t>Juego Sala- 123</t>
         </is>
       </c>
       <c r="C11" s="3" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D11" s="3" t="n">
-        <v>10</v>
+        <v>25.55</v>
       </c>
       <c r="E11" s="3" t="inlineStr">
         <is>
-          <t>unidad</t>
+          <t>juego</t>
         </is>
       </c>
       <c r="F11" s="3" t="inlineStr">
         <is>
-          <t>Comedor</t>
+          <t>Sala</t>
         </is>
       </c>
     </row>
@@ -732,23 +732,23 @@
       </c>
       <c r="B12" s="3" t="inlineStr">
         <is>
-          <t>bf12</t>
+          <t>...Afsbhehuhfhfdjkdsfjksjksdfjkfdjsfdhjsfd</t>
         </is>
       </c>
       <c r="C12" s="3" t="n">
         <v>12</v>
       </c>
       <c r="D12" s="3" t="n">
-        <v>25.55</v>
+        <v>111</v>
       </c>
       <c r="E12" s="3" t="inlineStr">
         <is>
-          <t>juego</t>
+          <t>kit</t>
         </is>
       </c>
       <c r="F12" s="3" t="inlineStr">
         <is>
-          <t>Sala</t>
+          <t>Comedor</t>
         </is>
       </c>
     </row>
@@ -758,18 +758,18 @@
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>...Afsbhehuhfhfdjkdsfjksjksdfjkfdjsfdhjsfd</t>
+          <t>pan</t>
         </is>
       </c>
       <c r="C13" s="3" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D13" s="3" t="n">
-        <v>111</v>
+        <v>10</v>
       </c>
       <c r="E13" s="3" t="inlineStr">
         <is>
-          <t>kit</t>
+          <t>unidad</t>
         </is>
       </c>
       <c r="F13" s="3" t="inlineStr">
@@ -784,14 +784,14 @@
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
-          <t>pan</t>
+          <t>Hola</t>
         </is>
       </c>
       <c r="C14" s="3" t="n">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="D14" s="3" t="n">
-        <v>10</v>
+        <v>123</v>
       </c>
       <c r="E14" s="3" t="inlineStr">
         <is>
@@ -810,14 +810,14 @@
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>Hola</t>
+          <t>Hola 123</t>
         </is>
       </c>
       <c r="C15" s="3" t="n">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="D15" s="3" t="n">
-        <v>123</v>
+        <v>12</v>
       </c>
       <c r="E15" s="3" t="inlineStr">
         <is>
@@ -826,7 +826,7 @@
       </c>
       <c r="F15" s="3" t="inlineStr">
         <is>
-          <t>Comedor</t>
+          <t>Sala</t>
         </is>
       </c>
     </row>
@@ -836,7 +836,7 @@
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>Hola 123</t>
+          <t>La Potona-</t>
         </is>
       </c>
       <c r="C16" s="3" t="n">
@@ -847,12 +847,12 @@
       </c>
       <c r="E16" s="3" t="inlineStr">
         <is>
-          <t>unidad</t>
+          <t>juego</t>
         </is>
       </c>
       <c r="F16" s="3" t="inlineStr">
         <is>
-          <t>Sala</t>
+          <t>Oficina</t>
         </is>
       </c>
     </row>
@@ -862,47 +862,21 @@
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>La Potona</t>
+          <t>Vas A Cáer Chuponsito</t>
         </is>
       </c>
       <c r="C17" s="3" t="n">
-        <v>12</v>
+        <v>1212</v>
       </c>
       <c r="D17" s="3" t="n">
         <v>12</v>
       </c>
       <c r="E17" s="3" t="inlineStr">
         <is>
-          <t>juego</t>
+          <t>par</t>
         </is>
       </c>
       <c r="F17" s="3" t="inlineStr">
-        <is>
-          <t>Oficina</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="3" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" s="3" t="inlineStr">
-        <is>
-          <t>Vas A Cáer Chuponsito</t>
-        </is>
-      </c>
-      <c r="C18" s="3" t="n">
-        <v>1212</v>
-      </c>
-      <c r="D18" s="3" t="n">
-        <v>12</v>
-      </c>
-      <c r="E18" s="3" t="inlineStr">
-        <is>
-          <t>par</t>
-        </is>
-      </c>
-      <c r="F18" s="3" t="inlineStr">
         <is>
           <t>Sala</t>
         </is>

</xml_diff>

<commit_message>
Bug 14 corregido- especificaciones al implementar excepciones
</commit_message>
<xml_diff>
--- a/reporte_inventario.xlsx
+++ b/reporte_inventario.xlsx
@@ -440,7 +440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,7 +456,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Reporte generado el 18/05/2025 a las 20:52</t>
+          <t>Reporte generado el 18/05/2025 a las 21:00</t>
         </is>
       </c>
     </row>
@@ -680,14 +680,14 @@
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
-          <t>Juego Sala - 123</t>
+          <t>Hola</t>
         </is>
       </c>
       <c r="C10" s="3" t="n">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="D10" s="3" t="n">
-        <v>1</v>
+        <v>123</v>
       </c>
       <c r="E10" s="3" t="inlineStr">
         <is>
@@ -706,177 +706,21 @@
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>Juego Sala- 123</t>
+          <t>Hola 123</t>
         </is>
       </c>
       <c r="C11" s="3" t="n">
         <v>12</v>
       </c>
       <c r="D11" s="3" t="n">
-        <v>25.55</v>
+        <v>12</v>
       </c>
       <c r="E11" s="3" t="inlineStr">
         <is>
-          <t>juego</t>
+          <t>unidad</t>
         </is>
       </c>
       <c r="F11" s="3" t="inlineStr">
-        <is>
-          <t>Sala</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" s="3" t="inlineStr">
-        <is>
-          <t>...Afsbhehuhfhfdjkdsfjksjksdfjkfdjsfdhjsfd</t>
-        </is>
-      </c>
-      <c r="C12" s="3" t="n">
-        <v>12</v>
-      </c>
-      <c r="D12" s="3" t="n">
-        <v>111</v>
-      </c>
-      <c r="E12" s="3" t="inlineStr">
-        <is>
-          <t>kit</t>
-        </is>
-      </c>
-      <c r="F12" s="3" t="inlineStr">
-        <is>
-          <t>Comedor</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="3" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" s="3" t="inlineStr">
-        <is>
-          <t>pan</t>
-        </is>
-      </c>
-      <c r="C13" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="D13" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="E13" s="3" t="inlineStr">
-        <is>
-          <t>unidad</t>
-        </is>
-      </c>
-      <c r="F13" s="3" t="inlineStr">
-        <is>
-          <t>Comedor</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="3" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" s="3" t="inlineStr">
-        <is>
-          <t>Hola</t>
-        </is>
-      </c>
-      <c r="C14" s="3" t="n">
-        <v>21</v>
-      </c>
-      <c r="D14" s="3" t="n">
-        <v>123</v>
-      </c>
-      <c r="E14" s="3" t="inlineStr">
-        <is>
-          <t>unidad</t>
-        </is>
-      </c>
-      <c r="F14" s="3" t="inlineStr">
-        <is>
-          <t>Comedor</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="3" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" s="3" t="inlineStr">
-        <is>
-          <t>Hola 123</t>
-        </is>
-      </c>
-      <c r="C15" s="3" t="n">
-        <v>12</v>
-      </c>
-      <c r="D15" s="3" t="n">
-        <v>12</v>
-      </c>
-      <c r="E15" s="3" t="inlineStr">
-        <is>
-          <t>unidad</t>
-        </is>
-      </c>
-      <c r="F15" s="3" t="inlineStr">
-        <is>
-          <t>Sala</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="3" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" s="3" t="inlineStr">
-        <is>
-          <t>La Potona-</t>
-        </is>
-      </c>
-      <c r="C16" s="3" t="n">
-        <v>12</v>
-      </c>
-      <c r="D16" s="3" t="n">
-        <v>12</v>
-      </c>
-      <c r="E16" s="3" t="inlineStr">
-        <is>
-          <t>juego</t>
-        </is>
-      </c>
-      <c r="F16" s="3" t="inlineStr">
-        <is>
-          <t>Oficina</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="3" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" s="3" t="inlineStr">
-        <is>
-          <t>Vas A Cáer Chuponsito</t>
-        </is>
-      </c>
-      <c r="C17" s="3" t="n">
-        <v>1212</v>
-      </c>
-      <c r="D17" s="3" t="n">
-        <v>12</v>
-      </c>
-      <c r="E17" s="3" t="inlineStr">
-        <is>
-          <t>par</t>
-        </is>
-      </c>
-      <c r="F17" s="3" t="inlineStr">
         <is>
           <t>Sala</t>
         </is>

</xml_diff>

<commit_message>
Ajustes finales para validar datos al ingresar productos
</commit_message>
<xml_diff>
--- a/reporte_inventario.xlsx
+++ b/reporte_inventario.xlsx
@@ -440,7 +440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,7 +456,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Reporte generado el 18/05/2025 a las 21:00</t>
+          <t>Reporte generado el 19/05/2025 a las 00:16</t>
         </is>
       </c>
     </row>
@@ -498,23 +498,23 @@
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>HPe</t>
+          <t>Cama Queen</t>
         </is>
       </c>
       <c r="C3" s="3" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D3" s="3" t="n">
-        <v>50</v>
+        <v>699</v>
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>pieza</t>
+          <t>unidad</t>
         </is>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>Sala</t>
+          <t>Dormitorio</t>
         </is>
       </c>
     </row>
@@ -524,23 +524,23 @@
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>Cama Queen</t>
+          <t>Juego de terraza</t>
         </is>
       </c>
       <c r="C4" s="3" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>699</v>
+        <v>899.9</v>
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>unidad</t>
+          <t>juego</t>
         </is>
       </c>
       <c r="F4" s="3" t="inlineStr">
         <is>
-          <t>Dormitorio</t>
+          <t>Exteriores</t>
         </is>
       </c>
     </row>
@@ -550,23 +550,23 @@
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>Juego de terraza</t>
+          <t>Lámpara de pie</t>
         </is>
       </c>
       <c r="C5" s="3" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="D5" s="3" t="n">
-        <v>899.9</v>
+        <v>85.75</v>
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>juego</t>
+          <t>unidad</t>
         </is>
       </c>
       <c r="F5" s="3" t="inlineStr">
         <is>
-          <t>Exteriores</t>
+          <t>Sala</t>
         </is>
       </c>
     </row>
@@ -576,14 +576,14 @@
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>Lámpara de pie</t>
+          <t>Escritorio ejecutivo</t>
         </is>
       </c>
       <c r="C6" s="3" t="n">
-        <v>15</v>
+        <v>10000000000</v>
       </c>
       <c r="D6" s="3" t="n">
-        <v>85.75</v>
+        <v>399</v>
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
@@ -592,7 +592,7 @@
       </c>
       <c r="F6" s="3" t="inlineStr">
         <is>
-          <t>Sala</t>
+          <t>Oficina</t>
         </is>
       </c>
     </row>
@@ -602,23 +602,23 @@
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>Escritorio ejecutivo</t>
+          <t>Velador doble</t>
         </is>
       </c>
       <c r="C7" s="3" t="n">
-        <v>10000000000</v>
+        <v>10</v>
       </c>
       <c r="D7" s="3" t="n">
-        <v>399</v>
+        <v>120</v>
       </c>
       <c r="E7" s="3" t="inlineStr">
         <is>
-          <t>unidad</t>
+          <t>par</t>
         </is>
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
-          <t>Oficina</t>
+          <t>Dormitorio</t>
         </is>
       </c>
     </row>
@@ -628,23 +628,23 @@
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>Velador doble</t>
+          <t>Silla comedor</t>
         </is>
       </c>
       <c r="C8" s="3" t="n">
-        <v>10</v>
+        <v>32000</v>
       </c>
       <c r="D8" s="3" t="n">
-        <v>120</v>
+        <v>45.999</v>
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t>par</t>
+          <t>unidad</t>
         </is>
       </c>
       <c r="F8" s="3" t="inlineStr">
         <is>
-          <t>Dormitorio</t>
+          <t>Exteriores</t>
         </is>
       </c>
     </row>
@@ -654,14 +654,14 @@
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>Silla comedor</t>
+          <t>Hola</t>
         </is>
       </c>
       <c r="C9" s="3" t="n">
-        <v>32000</v>
+        <v>21</v>
       </c>
       <c r="D9" s="3" t="n">
-        <v>45.999</v>
+        <v>123</v>
       </c>
       <c r="E9" s="3" t="inlineStr">
         <is>
@@ -670,7 +670,7 @@
       </c>
       <c r="F9" s="3" t="inlineStr">
         <is>
-          <t>Exteriores</t>
+          <t>Comedor</t>
         </is>
       </c>
     </row>
@@ -680,14 +680,14 @@
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
-          <t>Hola</t>
+          <t>Hola 123</t>
         </is>
       </c>
       <c r="C10" s="3" t="n">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="D10" s="3" t="n">
-        <v>123</v>
+        <v>12</v>
       </c>
       <c r="E10" s="3" t="inlineStr">
         <is>
@@ -696,7 +696,7 @@
       </c>
       <c r="F10" s="3" t="inlineStr">
         <is>
-          <t>Comedor</t>
+          <t>Sala</t>
         </is>
       </c>
     </row>
@@ -706,23 +706,75 @@
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>Hola 123</t>
+          <t>Sdf213</t>
         </is>
       </c>
       <c r="C11" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="D11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3" t="inlineStr">
+        <is>
+          <t>juego</t>
+        </is>
+      </c>
+      <c r="F11" s="3" t="inlineStr">
+        <is>
+          <t>Comedor</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t>Sad</t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="E12" s="3" t="inlineStr">
+        <is>
+          <t>juego</t>
+        </is>
+      </c>
+      <c r="F12" s="3" t="inlineStr">
+        <is>
+          <t>Oficina</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3" t="inlineStr">
+        <is>
+          <t>Sda</t>
+        </is>
+      </c>
+      <c r="C13" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="D11" s="3" t="n">
-        <v>12</v>
-      </c>
-      <c r="E11" s="3" t="inlineStr">
-        <is>
-          <t>unidad</t>
-        </is>
-      </c>
-      <c r="F11" s="3" t="inlineStr">
-        <is>
-          <t>Sala</t>
+      <c r="D13" s="3" t="n">
+        <v>2131232</v>
+      </c>
+      <c r="E13" s="3" t="inlineStr">
+        <is>
+          <t>par</t>
+        </is>
+      </c>
+      <c r="F13" s="3" t="inlineStr">
+        <is>
+          <t>Comedor</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Se cambia de id a n. a listas de pdf y excel para evitar confusiones
</commit_message>
<xml_diff>
--- a/reporte_inventario.xlsx
+++ b/reporte_inventario.xlsx
@@ -440,7 +440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,14 +456,14 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Reporte generado el 19/05/2025 a las 00:16</t>
+          <t>Reporte generado el 19/05/2025 a las 11:35</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>ID</t>
+          <t>N°.</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -498,23 +498,23 @@
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>Cama Queen</t>
+          <t>Mueble 123</t>
         </is>
       </c>
       <c r="C3" s="3" t="n">
-        <v>10</v>
+        <v>123</v>
       </c>
       <c r="D3" s="3" t="n">
-        <v>699</v>
+        <v>321</v>
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>unidad</t>
+          <t>juego</t>
         </is>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>Dormitorio</t>
+          <t>Sala</t>
         </is>
       </c>
     </row>
@@ -524,14 +524,14 @@
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>Juego de terraza</t>
+          <t>Boe 123</t>
         </is>
       </c>
       <c r="C4" s="3" t="n">
-        <v>3</v>
+        <v>43</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>899.9</v>
+        <v>35</v>
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
@@ -540,241 +540,7 @@
       </c>
       <c r="F4" s="3" t="inlineStr">
         <is>
-          <t>Exteriores</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" s="3" t="inlineStr">
-        <is>
-          <t>Lámpara de pie</t>
-        </is>
-      </c>
-      <c r="C5" s="3" t="n">
-        <v>15</v>
-      </c>
-      <c r="D5" s="3" t="n">
-        <v>85.75</v>
-      </c>
-      <c r="E5" s="3" t="inlineStr">
-        <is>
-          <t>unidad</t>
-        </is>
-      </c>
-      <c r="F5" s="3" t="inlineStr">
-        <is>
-          <t>Sala</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3" t="inlineStr">
-        <is>
-          <t>Escritorio ejecutivo</t>
-        </is>
-      </c>
-      <c r="C6" s="3" t="n">
-        <v>10000000000</v>
-      </c>
-      <c r="D6" s="3" t="n">
-        <v>399</v>
-      </c>
-      <c r="E6" s="3" t="inlineStr">
-        <is>
-          <t>unidad</t>
-        </is>
-      </c>
-      <c r="F6" s="3" t="inlineStr">
-        <is>
-          <t>Oficina</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" s="3" t="inlineStr">
-        <is>
-          <t>Velador doble</t>
-        </is>
-      </c>
-      <c r="C7" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="D7" s="3" t="n">
-        <v>120</v>
-      </c>
-      <c r="E7" s="3" t="inlineStr">
-        <is>
-          <t>par</t>
-        </is>
-      </c>
-      <c r="F7" s="3" t="inlineStr">
-        <is>
           <t>Dormitorio</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" s="3" t="inlineStr">
-        <is>
-          <t>Silla comedor</t>
-        </is>
-      </c>
-      <c r="C8" s="3" t="n">
-        <v>32000</v>
-      </c>
-      <c r="D8" s="3" t="n">
-        <v>45.999</v>
-      </c>
-      <c r="E8" s="3" t="inlineStr">
-        <is>
-          <t>unidad</t>
-        </is>
-      </c>
-      <c r="F8" s="3" t="inlineStr">
-        <is>
-          <t>Exteriores</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" s="3" t="inlineStr">
-        <is>
-          <t>Hola</t>
-        </is>
-      </c>
-      <c r="C9" s="3" t="n">
-        <v>21</v>
-      </c>
-      <c r="D9" s="3" t="n">
-        <v>123</v>
-      </c>
-      <c r="E9" s="3" t="inlineStr">
-        <is>
-          <t>unidad</t>
-        </is>
-      </c>
-      <c r="F9" s="3" t="inlineStr">
-        <is>
-          <t>Comedor</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="3" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" s="3" t="inlineStr">
-        <is>
-          <t>Hola 123</t>
-        </is>
-      </c>
-      <c r="C10" s="3" t="n">
-        <v>12</v>
-      </c>
-      <c r="D10" s="3" t="n">
-        <v>12</v>
-      </c>
-      <c r="E10" s="3" t="inlineStr">
-        <is>
-          <t>unidad</t>
-        </is>
-      </c>
-      <c r="F10" s="3" t="inlineStr">
-        <is>
-          <t>Sala</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="3" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" s="3" t="inlineStr">
-        <is>
-          <t>Sdf213</t>
-        </is>
-      </c>
-      <c r="C11" s="3" t="n">
-        <v>23</v>
-      </c>
-      <c r="D11" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" s="3" t="inlineStr">
-        <is>
-          <t>juego</t>
-        </is>
-      </c>
-      <c r="F11" s="3" t="inlineStr">
-        <is>
-          <t>Comedor</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" s="3" t="inlineStr">
-        <is>
-          <t>Sad</t>
-        </is>
-      </c>
-      <c r="C12" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" s="3" t="n">
-        <v>23</v>
-      </c>
-      <c r="E12" s="3" t="inlineStr">
-        <is>
-          <t>juego</t>
-        </is>
-      </c>
-      <c r="F12" s="3" t="inlineStr">
-        <is>
-          <t>Oficina</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="3" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" s="3" t="inlineStr">
-        <is>
-          <t>Sda</t>
-        </is>
-      </c>
-      <c r="C13" s="3" t="n">
-        <v>12</v>
-      </c>
-      <c r="D13" s="3" t="n">
-        <v>2131232</v>
-      </c>
-      <c r="E13" s="3" t="inlineStr">
-        <is>
-          <t>par</t>
-        </is>
-      </c>
-      <c r="F13" s="3" t="inlineStr">
-        <is>
-          <t>Comedor</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Ajustes de ancho en columna en generacion de informe en excel
</commit_message>
<xml_diff>
--- a/reporte_inventario.xlsx
+++ b/reporte_inventario.xlsx
@@ -33,12 +33,17 @@
       <color rgb="00FFFFFF"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="001976D2"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -64,12 +69,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -440,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,15 +456,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="35" customWidth="1" min="2" max="2"/>
-    <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="18" customWidth="1" min="6" max="6"/>
+    <col width="10" customWidth="1" min="1" max="1"/>
+    <col width="10" customWidth="1" min="2" max="2"/>
+    <col width="35" customWidth="1" min="3" max="3"/>
+    <col width="26" customWidth="1" min="4" max="4"/>
+    <col width="26" customWidth="1" min="5" max="5"/>
+    <col width="26" customWidth="1" min="6" max="6"/>
+    <col width="25" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Reporte generado el 19/05/2025 a las 11:35</t>
+          <t>Reporte generado el 19/05/2025 a las 11:56</t>
         </is>
       </c>
     </row>
@@ -466,81 +478,121 @@
           <t>N°.</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
         <is>
           <t>Nombre</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="D2" s="3" t="inlineStr">
         <is>
           <t>Cantidad</t>
         </is>
       </c>
-      <c r="D2" s="2" t="inlineStr">
+      <c r="E2" s="3" t="inlineStr">
         <is>
           <t>Precio</t>
         </is>
       </c>
-      <c r="E2" s="2" t="inlineStr">
+      <c r="F2" s="3" t="inlineStr">
         <is>
           <t>Unidad</t>
         </is>
       </c>
-      <c r="F2" s="2" t="inlineStr">
+      <c r="G2" s="3" t="inlineStr">
         <is>
           <t>Categoría</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="n">
+      <c r="A3" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="inlineStr">
+      <c r="B3" s="4" t="n">
+        <v>62</v>
+      </c>
+      <c r="C3" s="4" t="inlineStr">
         <is>
           <t>Mueble 123</t>
         </is>
       </c>
-      <c r="C3" s="3" t="n">
+      <c r="D3" s="4" t="n">
         <v>123</v>
       </c>
-      <c r="D3" s="3" t="n">
+      <c r="E3" s="4" t="n">
         <v>321</v>
       </c>
-      <c r="E3" s="3" t="inlineStr">
+      <c r="F3" s="4" t="inlineStr">
         <is>
           <t>juego</t>
         </is>
       </c>
-      <c r="F3" s="3" t="inlineStr">
+      <c r="G3" s="4" t="inlineStr">
         <is>
           <t>Sala</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="n">
+      <c r="A4" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="inlineStr">
+      <c r="B4" s="4" t="n">
+        <v>63</v>
+      </c>
+      <c r="C4" s="4" t="inlineStr">
         <is>
           <t>Boe 123</t>
         </is>
       </c>
-      <c r="C4" s="3" t="n">
+      <c r="D4" s="4" t="n">
         <v>43</v>
       </c>
-      <c r="D4" s="3" t="n">
+      <c r="E4" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="E4" s="3" t="inlineStr">
+      <c r="F4" s="4" t="inlineStr">
         <is>
           <t>juego</t>
         </is>
       </c>
-      <c r="F4" s="3" t="inlineStr">
+      <c r="G4" s="4" t="inlineStr">
         <is>
           <t>Dormitorio</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4" t="n">
+        <v>64</v>
+      </c>
+      <c r="C5" s="4" t="inlineStr">
+        <is>
+          <t>Oeoeoeoeoeoeoeoeoeoe</t>
+        </is>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="E5" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="F5" s="4" t="inlineStr">
+        <is>
+          <t>par</t>
+        </is>
+      </c>
+      <c r="G5" s="4" t="inlineStr">
+        <is>
+          <t>Sala</t>
         </is>
       </c>
     </row>

</xml_diff>